<commit_message>
final touch for browser management
</commit_message>
<xml_diff>
--- a/CucumberCraft/src/test/resources/Fixture/Promo_DB_Data.xlsx
+++ b/CucumberCraft/src/test/resources/Fixture/Promo_DB_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="121">
   <si>
     <t>Test Scenario</t>
   </si>
@@ -815,7 +815,7 @@
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,9 +877,7 @@
       <c r="D2" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -902,9 +900,7 @@
       <c r="D3" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -927,9 +923,7 @@
       <c r="D4" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -952,9 +946,7 @@
       <c r="D5" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1635,9 +1627,7 @@
       <c r="D31" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>77</v>
-      </c>
+      <c r="E31" s="7"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>

</xml_diff>